<commit_message>
update copyright year to 2021 in printable matrix
</commit_message>
<xml_diff>
--- a/Telematics Cybersecurity Requirements Matrix.xlsx
+++ b/Telematics Cybersecurity Requirements Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Gardiner\src\nmfta-telematics_security_requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADF230B-C7F4-4029-A9D9-D4EEDE0FE196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F0C900-2369-41CF-980E-AAAACB96A8C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8595" yWindow="-21600" windowWidth="54885" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8760" yWindow="-21720" windowWidth="77040" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matrix" sheetId="1" r:id="rId1"/>
@@ -4024,7 +4024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7248,7 +7248,7 @@
   <dimension ref="A1:H780"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="16.75" x14ac:dyDescent="0.45"/>
@@ -22091,7 +22091,7 @@
   <headerFooter>
     <oddHeader>&amp;L&amp;G
 Source: &amp;U&amp;K0070C0https://github.com/nmfta-repo/nmfta-telematics_security_requirements</oddHeader>
-    <oddFooter>&amp;L&amp;9&amp;K002060National Motor Freight Traffic Association, Inc.&amp;C&amp;9&amp;K002060© 2020 All Rights Reserved &amp;R&amp;9&amp;K02-049Page | &amp;P – Appendix A</oddFooter>
+    <oddFooter>&amp;L&amp;9&amp;K002060National Motor Freight Traffic Association, Inc.&amp;C&amp;9&amp;K002060© 2021 All Rights Reserved &amp;R&amp;9&amp;K02-047Page | &amp;P – Appendix A</oddFooter>
   </headerFooter>
   <rowBreaks count="70" manualBreakCount="70">
     <brk id="10" max="16383" man="1"/>

</xml_diff>

<commit_message>
homing the excel cursor
</commit_message>
<xml_diff>
--- a/Telematics Cybersecurity Requirements Matrix.xlsx
+++ b/Telematics Cybersecurity Requirements Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben Gardiner\src\nmfta-telematics_security_requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED2E00E-0643-4F79-896A-B99F0F383E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944CEB2D-3BDA-4E6E-8C6D-F12C0995468E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" tabRatio="464" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4069,10 +4069,10 @@
   <dimension ref="A1:M72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E60" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E61" sqref="E61"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>

</xml_diff>